<commit_message>
update check staff and import excel
</commit_message>
<xml_diff>
--- a/ERP.API/TempFiles/2020-02-19/department_200219165142.xlsx
+++ b/ERP.API/TempFiles/2020-02-19/department_200219165142.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BootAi\ERP20\ERP.API\TempFiles\2020-02-19\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ERP20\ERP.API\TempFiles\2020-02-19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1862334F-BDA6-468B-A817-0F0207CE2426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A352558E-BC24-4956-90BA-A0213A912CAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11145" yWindow="2970" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Staffs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>trungtn</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>Hà nội</t>
-  </si>
-  <si>
-    <t>Nam</t>
   </si>
   <si>
     <t>sta_fullname</t>
@@ -89,7 +86,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -97,6 +94,13 @@
     <font>
       <sz val="10"/>
       <name val="Calibiri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,15 +120,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="47" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -454,51 +461,52 @@
     <col min="10" max="10" width="9.140625" style="1" customWidth="1"/>
     <col min="11" max="11" width="12.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="13" width="19.85546875" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" ht="15">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -506,7 +514,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -514,7 +522,7 @@
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -526,8 +534,8 @@
       <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>6</v>
+      <c r="J2" s="1">
+        <v>1</v>
       </c>
       <c r="K2" s="2">
         <v>43040</v>
@@ -539,7 +547,53 @@
         <v>43040</v>
       </c>
     </row>
+    <row r="3" spans="1:13" ht="15">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2">
+        <v>43040</v>
+      </c>
+      <c r="L3" s="1">
+        <v>80809</v>
+      </c>
+      <c r="M3" s="2">
+        <v>43040</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{F8EDF866-CBFC-4D52-AFAD-F552B4819050}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{BE917424-D75A-4CAF-98D2-4B141C19B15B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>